<commit_message>
implementando roles y modulos
</commit_message>
<xml_diff>
--- a/public/formatos/descuento_import.xlsx
+++ b/public/formatos/descuento_import.xlsx
@@ -20,15 +20,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t xml:space="preserve">numero_de_documento</t>
   </si>
   <si>
+    <t xml:space="preserve">categoria</t>
+  </si>
+  <si>
     <t xml:space="preserve">descuento</t>
   </si>
   <si>
     <t xml:space="preserve">monto</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Guía para una importación exitosa   ***</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFCC0000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Eliminar esta tabla a la hora importar</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">***</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Columna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requerido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requerido, en este campo se debe de ingresar el identificador del la categoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requerido, en este campo se debe de ingresar el identificador del descuento</t>
   </si>
 </sst>
 </file>
@@ -38,7 +91,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -60,6 +113,22 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,13 +180,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -129,6 +210,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -137,18 +278,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="3" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -161,8 +302,77 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>